<commit_message>
Se agrego un snippet de reflexion
</commit_message>
<xml_diff>
--- a/testVSTO2/Resources/FICHA RECETA.xlsx
+++ b/testVSTO2/Resources/FICHA RECETA.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Receta" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="ReporteInventario" sheetId="3" r:id="rId2"/>
+    <sheet name="ReporteInventarioImprimir" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="CANTIDAD_A_ELABORAR">Receta!$J$4</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Receta</t>
   </si>
@@ -133,6 +135,100 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Clave</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Producto     </t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Inventario Sistema</t>
+  </si>
+  <si>
+    <t>Consumo Diario Promedio</t>
+  </si>
+  <si>
+    <t>Punto de 
+Re-ORDEN</t>
+  </si>
+  <si>
+    <t>Cantidad Articulos
+Vendidos</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>Fecha  Ultima Compra</t>
+  </si>
+  <si>
+    <t>Cantidad Comprada</t>
+  </si>
+  <si>
+    <t>Precio de Compra</t>
+  </si>
+  <si>
+    <t>Precio Venta</t>
+  </si>
+  <si>
+    <t>Margen</t>
+  </si>
+  <si>
+    <t>Radio
+Inventario</t>
+  </si>
+  <si>
+    <t>Existencia Sistema</t>
+  </si>
+  <si>
+    <t>Cantidad a PEDIR</t>
+  </si>
+  <si>
+    <t>Coca Cola 600 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-1  </t>
+  </si>
+  <si>
+    <t>Semanal</t>
+  </si>
+  <si>
+    <t>Inv. 
+Min.</t>
+  </si>
+  <si>
+    <t>Inv. Máx.</t>
+  </si>
+  <si>
+    <t>Factor Compra</t>
+  </si>
+  <si>
+    <t>Fecha:</t>
+  </si>
+  <si>
+    <t>Almacenes Mercatto S. de R.L. de C.V.</t>
+  </si>
+  <si>
+    <t>Pedido</t>
+  </si>
+  <si>
+    <t>Inv. Min</t>
+  </si>
+  <si>
+    <t>Inv. Max</t>
+  </si>
+  <si>
+    <t>FACTOR(Presentación de Compra)</t>
   </si>
 </sst>
 </file>
@@ -143,7 +239,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,8 +308,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,8 +371,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -567,6 +712,173 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -575,7 +887,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -652,6 +964,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -729,13 +1123,101 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -746,11 +1228,6 @@
         <b/>
         <i val="0"/>
         <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
       </font>
     </dxf>
   </dxfs>
@@ -764,6 +1241,83 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>253596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="428625" y="0"/>
+          <a:ext cx="1276350" cy="634596"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:S1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:S1048576"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="Clave"/>
+    <tableColumn id="2" name="Departamento"/>
+    <tableColumn id="3" name="Categoria"/>
+    <tableColumn id="4" name="Producto     "/>
+    <tableColumn id="5" name="Tipo"/>
+    <tableColumn id="6" name="Inventario Sistema"/>
+    <tableColumn id="7" name="Consumo Diario Promedio"/>
+    <tableColumn id="8" name="Punto de _x000a_Re-ORDEN"/>
+    <tableColumn id="9" name="Inv. Min"/>
+    <tableColumn id="10" name="Inv. Max"/>
+    <tableColumn id="11" name="FACTOR(Presentación de Compra)"/>
+    <tableColumn id="12" name="Cantidad Articulos_x000a_Vendidos"/>
+    <tableColumn id="13" name="Ventas"/>
+    <tableColumn id="14" name="Fecha  Ultima Compra"/>
+    <tableColumn id="15" name="Cantidad Comprada"/>
+    <tableColumn id="16" name="Radio_x000a_Inventario"/>
+    <tableColumn id="17" name="Precio de Compra"/>
+    <tableColumn id="18" name="Precio Venta"/>
+    <tableColumn id="19" name="Margen" dataCellStyle="Porcentaje"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1055,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1073,50 +1627,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67"/>
       <c r="G1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="75"/>
+      <c r="B2" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="29" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="34"/>
+      <c r="I2" s="62"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="33" t="s">
+      <c r="A3" s="76"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="62"/>
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1141,10 +1695,10 @@
       <c r="G4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="36"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1158,10 +1712,10 @@
         <f t="shared" ref="G5:G11" si="0">C5*F5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="32"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="9">
         <f>SUM(G5:G100)</f>
         <v>0</v>
@@ -1178,10 +1732,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="60"/>
       <c r="J6" s="10">
         <f>J5*0.05</f>
         <v>0</v>
@@ -1198,10 +1752,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="60"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1215,10 +1769,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="60"/>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1232,10 +1786,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="59"/>
       <c r="J9" s="19">
         <f>(PRECIO_VENTA*LITROS_A_ELABORAR)</f>
         <v>0</v>
@@ -1252,10 +1806,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="59"/>
       <c r="J10" s="20">
         <f>J9-COSTO_TOTAL_MATERIA_PRIMA</f>
         <v>0</v>
@@ -1272,10 +1826,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="28"/>
+      <c r="I11" s="56"/>
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
@@ -1289,10 +1843,10 @@
         <f t="shared" ref="G12:G18" si="1">C12*F12</f>
         <v>0</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="28"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="18" t="e">
         <f>(J5/J9-1)*(-1)</f>
         <v>#DIV/0!</v>
@@ -1399,10 +1953,10 @@
     <mergeCell ref="H11:I11"/>
   </mergeCells>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>$J$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>$J$11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1412,6 +1966,297 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="90"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="83" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="86" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="86" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="89" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="81">
+        <v>42491</v>
+      </c>
+      <c r="I1" s="81"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+    </row>
+    <row r="3" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="54"/>
+      <c r="C3" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+    </row>
+    <row r="4" spans="1:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="34">
+        <v>15</v>
+      </c>
+      <c r="D5" s="35">
+        <v>5.8</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="37">
+        <v>41</v>
+      </c>
+      <c r="G5" s="36">
+        <v>59</v>
+      </c>
+      <c r="H5" s="37">
+        <v>24</v>
+      </c>
+      <c r="I5" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="44"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:I3"/>
+  </mergeCells>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Bloqueo y desbloqueo para sortear filas
</commit_message>
<xml_diff>
--- a/testVSTO2/Resources/FICHA RECETA.xlsx
+++ b/testVSTO2/Resources/FICHA RECETA.xlsx
@@ -16,6 +16,7 @@
     <sheet name="ReporteInventario" sheetId="3" r:id="rId2"/>
     <sheet name="ReporteInventarioImprimir" sheetId="4" r:id="rId3"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="CANTIDAD_A_ELABORAR">Receta!$J$4</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Receta</t>
   </si>
@@ -104,9 +105,6 @@
     <t>Costo Total de Preparación</t>
   </si>
   <si>
-    <t>[NOMBRE]</t>
-  </si>
-  <si>
     <t>Cantidad Unitaria</t>
   </si>
   <si>
@@ -132,9 +130,6 @@
   </si>
   <si>
     <t>Margen actual</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Clave</t>
@@ -228,7 +223,22 @@
     <t>Inv. Max</t>
   </si>
   <si>
-    <t>FACTOR(Presentación de Compra)</t>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>CEBICHE</t>
+  </si>
+  <si>
+    <t>ce001</t>
+  </si>
+  <si>
+    <t>CEBOLLA BLANCA</t>
+  </si>
+  <si>
+    <t>CILANTRO</t>
+  </si>
+  <si>
+    <t>CAMARON FRESCO</t>
   </si>
 </sst>
 </file>
@@ -887,7 +897,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1046,6 +1056,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1141,83 +1172,44 @@
     <xf numFmtId="14" fontId="8" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="10" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1290,34 +1282,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:S1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:S1048576"/>
-  <tableColumns count="19">
-    <tableColumn id="1" name="Clave"/>
-    <tableColumn id="2" name="Departamento"/>
-    <tableColumn id="3" name="Categoria"/>
-    <tableColumn id="4" name="Producto     "/>
-    <tableColumn id="5" name="Tipo"/>
-    <tableColumn id="6" name="Inventario Sistema"/>
-    <tableColumn id="7" name="Consumo Diario Promedio"/>
-    <tableColumn id="8" name="Punto de _x000a_Re-ORDEN"/>
-    <tableColumn id="9" name="Inv. Min"/>
-    <tableColumn id="10" name="Inv. Max"/>
-    <tableColumn id="11" name="FACTOR(Presentación de Compra)"/>
-    <tableColumn id="12" name="Cantidad Articulos_x000a_Vendidos"/>
-    <tableColumn id="13" name="Ventas"/>
-    <tableColumn id="14" name="Fecha  Ultima Compra"/>
-    <tableColumn id="15" name="Cantidad Comprada"/>
-    <tableColumn id="16" name="Radio_x000a_Inventario"/>
-    <tableColumn id="17" name="Precio de Compra"/>
-    <tableColumn id="18" name="Precio Venta"/>
-    <tableColumn id="19" name="Margen" dataCellStyle="Porcentaje"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1610,7 +1574,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1627,61 +1591,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="65" t="s">
+      <c r="A1" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="67"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="75"/>
-      <c r="B2" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="61" t="s">
+      <c r="A2" s="82"/>
+      <c r="B2" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="12"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="12">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="61" t="s">
+      <c r="A3" s="83"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="13"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="13">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>22</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>3</v>
@@ -1695,85 +1663,126 @@
       <c r="G4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="14"/>
+      <c r="H4" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="71"/>
+      <c r="J4" s="14">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="A5" s="6">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="22">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="7">
+        <v>7.45</v>
+      </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G11" si="0">C5*F5</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="59" t="s">
+        <v>29.8</v>
+      </c>
+      <c r="H5" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="60"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="9">
         <f>SUM(G5:G100)</f>
-        <v>0</v>
+        <v>892</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="6">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="G6" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="59" t="s">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H6" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="60"/>
+      <c r="I6" s="67"/>
       <c r="J6" s="10">
         <f>J5*0.05</f>
-        <v>0</v>
+        <v>44.6</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="A7" s="6">
+        <v>178</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="22">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="7">
+        <v>215</v>
+      </c>
       <c r="G7" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="59" t="s">
+        <v>860</v>
+      </c>
+      <c r="H7" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="60"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="10">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="22"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6">
+        <v>5</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G8:G11" si="0">C8*F8</f>
         <v>0</v>
       </c>
-      <c r="H8" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="11"/>
+      <c r="H8" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="67"/>
+      <c r="J8" s="11">
+        <v>150</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
@@ -1786,13 +1795,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="59"/>
+      <c r="H9" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="66"/>
       <c r="J9" s="19">
         <f>(PRECIO_VENTA*LITROS_A_ELABORAR)</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1806,13 +1815,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="59"/>
+      <c r="H10" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="66"/>
       <c r="J10" s="20">
         <f>J9-COSTO_TOTAL_MATERIA_PRIMA</f>
-        <v>0</v>
+        <v>608</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
@@ -1826,11 +1835,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="56"/>
-      <c r="J11" s="18"/>
+      <c r="H11" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="63"/>
+      <c r="J11" s="18">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1843,13 +1854,13 @@
         <f t="shared" ref="G12:G18" si="1">C12*F12</f>
         <v>0</v>
       </c>
-      <c r="H12" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="56"/>
-      <c r="J12" s="18" t="e">
+      <c r="H12" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="63"/>
+      <c r="J12" s="18">
         <f>(J5/J9-1)*(-1)</f>
-        <v>#DIV/0!</v>
+        <v>0.40533333333333332</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1953,10 +1964,10 @@
     <mergeCell ref="H11:I11"/>
   </mergeCells>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>$J$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>$J$11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1970,93 +1981,81 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="90"/>
+    <col min="1" max="5" width="11.42578125" style="93"/>
+    <col min="6" max="13" width="11.42578125" style="98"/>
+    <col min="14" max="14" width="11.42578125" style="100"/>
+    <col min="15" max="18" width="11.42578125" style="98"/>
+    <col min="19" max="19" width="11.42578125" style="102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:19" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="D1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="E1" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="F1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="G1" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="H1" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="I1" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="85" t="s">
+      <c r="M1" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="85" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" s="86" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="87" t="s">
+      <c r="N1" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="88" t="s">
+      <c r="O1" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="86" t="s">
+      <c r="P1" s="95" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="85" t="s">
+      <c r="R1" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="85" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="86" t="s">
+      <c r="S1" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="85" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="89" t="s">
-        <v>45</v>
-      </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -2065,7 +2064,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,78 +2081,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="81">
+      <c r="B1" s="84" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="88">
         <v>42491</v>
       </c>
-      <c r="I1" s="81"/>
+      <c r="I1" s="88"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
     </row>
     <row r="3" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="54"/>
-      <c r="C3" s="78" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
+      <c r="C3" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
       <c r="F3" s="54"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
     </row>
     <row r="4" spans="1:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>37</v>
-      </c>
       <c r="E4" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>54</v>
-      </c>
       <c r="I4" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="34">
         <v>15</v>
@@ -2162,7 +2161,7 @@
         <v>5.8</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="37">
         <v>41</v>
@@ -2404,4 +2403,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cambios fuertes en los sidebars, se hacen validaciones de double en los inputs
</commit_message>
<xml_diff>
--- a/testVSTO2/Resources/FICHA RECETA.xlsx
+++ b/testVSTO2/Resources/FICHA RECETA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Receta" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <definedName name="CODIGO">Receta!$G$2</definedName>
     <definedName name="COSTO_PREPARACION">Receta!$J$7</definedName>
     <definedName name="COSTO_TOTAL_MATERIA_PRIMA">Receta!$J$5</definedName>
+    <definedName name="FECHA_FIN_IMP">ReporteInventarioImprimir!$H$2</definedName>
+    <definedName name="FECHA_INI_IMP">ReporteInventarioImprimir!$H$1</definedName>
     <definedName name="LITROS_A_ELABORAR">Receta!$J$3</definedName>
     <definedName name="MARGEN_ANTERIOR">Receta!$J$11</definedName>
     <definedName name="MARGEN_PRODUCTO">Receta!$J$12</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>Receta</t>
   </si>
@@ -202,15 +204,9 @@
     <t>Factor Compra</t>
   </si>
   <si>
-    <t>Fecha:</t>
-  </si>
-  <si>
     <t>Almacenes Mercatto S. de R.L. de C.V.</t>
   </si>
   <si>
-    <t>Pedido</t>
-  </si>
-  <si>
     <t>Inv. Min</t>
   </si>
   <si>
@@ -226,16 +222,34 @@
     <t>ce001</t>
   </si>
   <si>
-    <t>CEBOLLA BLANCA</t>
-  </si>
-  <si>
-    <t>CILANTRO</t>
-  </si>
-  <si>
-    <t>CAMARON FRESCO</t>
-  </si>
-  <si>
     <t>P-1</t>
+  </si>
+  <si>
+    <t>Inventario CEDIS</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Fecha I:</t>
+  </si>
+  <si>
+    <t>Fecha F:</t>
+  </si>
+  <si>
+    <t>PEDIDO DE COMPRA</t>
   </si>
 </sst>
 </file>
@@ -246,7 +260,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +360,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +418,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -879,7 +907,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,257 +933,50 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="10" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1171,18 +992,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1191,24 +1000,327 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1256,7 +1368,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1704975</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>253596</xdr:rowOff>
+      <xdr:rowOff>177396</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1581,367 +1693,291 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="20" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="29" style="20" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="20" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="15" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58"/>
-      <c r="B2" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="65" t="s">
+      <c r="A2" s="106"/>
+      <c r="B2" s="99" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="66"/>
-      <c r="J2" s="12">
+      <c r="I2" s="93"/>
+      <c r="J2" s="36">
         <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="65" t="s">
+      <c r="A3" s="107"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="13">
+      <c r="I3" s="93"/>
+      <c r="J3" s="37">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="68"/>
-      <c r="J4" s="14">
+      <c r="I4" s="95"/>
+      <c r="J4" s="40">
         <v>8.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="C5" s="22">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="7">
-        <v>7.45</v>
-      </c>
-      <c r="G5" s="7">
-        <v>29.8</v>
-      </c>
-      <c r="H5" s="56" t="s">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="9">
+      <c r="I5" s="91"/>
+      <c r="J5" s="44">
         <f>SUM(G5:G100)</f>
-        <v>892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C6" s="22">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G6" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="10">
+      <c r="I6" s="91"/>
+      <c r="J6" s="45">
         <f>J5*0.05</f>
-        <v>44.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>178</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="C7" s="22">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="7">
-        <v>215</v>
-      </c>
-      <c r="G7" s="7">
-        <v>860</v>
-      </c>
-      <c r="H7" s="56" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="60"/>
-      <c r="J7" s="10">
+      <c r="I7" s="91"/>
+      <c r="J7" s="45">
         <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="6">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7">
-        <f t="shared" ref="G8:G11" si="0">C8*F8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="56" t="s">
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="11">
+      <c r="I8" s="91"/>
+      <c r="J8" s="46">
         <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="56" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="56"/>
-      <c r="J9" s="19">
+      <c r="I9" s="90"/>
+      <c r="J9" s="47">
         <f>(PRECIO_VENTA*LITROS_A_ELABORAR)</f>
         <v>1500</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="56" t="s">
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="56"/>
-      <c r="J10" s="20">
+      <c r="I10" s="90"/>
+      <c r="J10" s="48">
         <f>J9-COSTO_TOTAL_MATERIA_PRIMA</f>
-        <v>608</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="61" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="62"/>
-      <c r="J11" s="18">
+      <c r="I11" s="87"/>
+      <c r="J11" s="49">
         <v>0.27</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7">
-        <f t="shared" ref="G12:G18" si="1">C12*F12</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="61" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="62"/>
-      <c r="J12" s="18">
-        <f>(J5/J9-1)*(-1)</f>
-        <v>0.40533333333333332</v>
+      <c r="I12" s="87"/>
+      <c r="J12" s="49">
+        <f>((J5+COSTO_PREPARACION)/J9-1)*(-1)</f>
+        <v>0.92666666666666664</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="43"/>
+    </row>
+    <row r="16" spans="1:10" s="51" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="43"/>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="43"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="43"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
@@ -1955,6 +1991,13 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="15">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H5:I5"/>
@@ -1963,13 +2006,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="J12">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
@@ -1986,78 +2022,151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="11.42578125" style="37"/>
-    <col min="6" max="13" width="11.42578125" style="42"/>
-    <col min="14" max="14" width="11.42578125" style="44"/>
-    <col min="15" max="18" width="11.42578125" style="42"/>
-    <col min="19" max="19" width="11.42578125" style="46"/>
+    <col min="1" max="4" width="11.42578125" style="55"/>
+    <col min="5" max="5" width="11.42578125" style="34"/>
+    <col min="6" max="6" width="11.42578125" style="58"/>
+    <col min="7" max="7" width="12.140625" style="58" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="58"/>
+    <col min="10" max="11" width="11.42578125" style="35"/>
+    <col min="12" max="14" width="11.42578125" style="58"/>
+    <col min="15" max="15" width="11.42578125" style="62"/>
+    <col min="16" max="18" width="11.42578125" style="58"/>
+    <col min="19" max="19" width="11.42578125" style="35"/>
+    <col min="20" max="20" width="11.42578125" style="58"/>
+    <col min="21" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:20" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="I1" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="N1" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="43" t="s">
+      <c r="O1" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="P1" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="Q1" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="R1" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="S1" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="T1" s="63" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="58">
+        <v>5</v>
+      </c>
+      <c r="G2" s="58">
+        <v>6</v>
+      </c>
+      <c r="H2" s="58">
+        <v>7</v>
+      </c>
+      <c r="I2" s="58">
+        <v>8</v>
+      </c>
+      <c r="J2" s="35">
+        <v>9</v>
+      </c>
+      <c r="K2" s="35">
+        <v>10</v>
+      </c>
+      <c r="L2" s="58">
+        <v>11</v>
+      </c>
+      <c r="M2" s="58">
+        <v>12</v>
+      </c>
+      <c r="N2" s="58">
+        <v>13</v>
+      </c>
+      <c r="O2" s="62">
+        <v>14</v>
+      </c>
+      <c r="P2" s="58">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="58">
+        <v>16</v>
+      </c>
+      <c r="R2" s="58">
+        <v>17</v>
+      </c>
+      <c r="S2" s="35">
+        <v>18</v>
+      </c>
+      <c r="T2" s="58">
+        <f>((R2/L2)/S2)*-1</f>
+        <v>-8.5858585858585856E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2069,120 +2178,124 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="69" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="69" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="69" customWidth="1"/>
-    <col min="4" max="4" width="11" style="69" customWidth="1"/>
-    <col min="5" max="5" width="9" style="69" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="69" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="69" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="69" customWidth="1"/>
-    <col min="9" max="9" width="8" style="69" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="69"/>
+    <col min="1" max="1" width="31.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="35" customWidth="1"/>
+    <col min="4" max="4" width="11" style="35" customWidth="1"/>
+    <col min="5" max="5" width="9" style="20" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="8" style="35" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="35" customWidth="1"/>
+    <col min="9" max="9" width="8" style="20" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71" t="s">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="72">
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="110">
         <v>42491</v>
       </c>
-      <c r="I1" s="72"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-    </row>
-    <row r="3" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="73"/>
-      <c r="C3" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-    </row>
-    <row r="4" spans="1:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="I1" s="110"/>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="110">
+        <v>42639</v>
+      </c>
+      <c r="I2" s="110"/>
+    </row>
+    <row r="3" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="108" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+    </row>
+    <row r="4" spans="1:10" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="81" t="s">
+      <c r="G4" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="79" t="s">
+      <c r="H4" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="82" t="s">
+      <c r="I4" s="81" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="83" t="s">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="100" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="84">
+      <c r="B5" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="64">
         <v>15</v>
       </c>
-      <c r="D5" s="85">
+      <c r="D5" s="65">
         <v>5.8</v>
       </c>
-      <c r="E5" s="86" t="str">
+      <c r="E5" s="22" t="str">
         <f>IF(B5="P-.5","Semanal",IF(B5="P-1","Semanal",IF(B5=1,ROUNDUP(F5+(D5*2),0),IF(B5=4,ROUNDUP(F5/2,0),"N/A"))))</f>
         <v>Semanal</v>
       </c>
-      <c r="F5" s="87">
+      <c r="F5" s="73">
         <v>41</v>
       </c>
-      <c r="G5" s="86">
+      <c r="G5" s="74">
         <v>54</v>
       </c>
-      <c r="H5" s="87">
+      <c r="H5" s="73">
         <v>24</v>
       </c>
-      <c r="I5" s="88">
+      <c r="I5" s="23">
         <f>IF(B5="P-.5",
 ODD((G5-C5)/H5),
 IF(B5="P-1",
@@ -2192,20 +2305,24 @@
 "PEDIDO DESCONOCIDO"))))</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="89"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="86" t="str">
+      <c r="J5" s="20">
+        <f>IF(B5=4,_xlfn.CEILING.MATH(396,12),IF(B5=1,_xlfn.CEILING.MATH(168,12),IF(B5="P-1",_xlfn.CEILING.MATH(126,12),IF(B5="P-.5",_xlfn.CEILING.MATH(108,12)))))</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="22" t="str">
         <f>IF(B6="P-.5","Semanal",IF(B6="P-1","Semanal",IF(B6=1,ROUNDUP(F6+(D6*2),0),IF(B6=4,ROUNDUP(F6/2,0),"N/A"))))</f>
         <v>N/A</v>
       </c>
-      <c r="F6" s="93"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="88" t="str">
+      <c r="F6" s="68"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="23" t="str">
         <f>IF(B6="P-.5",
 ODD((G6-C6)/H6),
 IF(B6="P-1",
@@ -2216,19 +2333,19 @@
         <v>PEDIDO DESCONOCIDO</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="86" t="str">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="22" t="str">
         <f t="shared" ref="E7:E11" si="0">IF(B7="P-.5","Semanal",IF(B7="P-1","Semanal",IF(B7=1,ROUNDUP(F7+(D7*2),0),IF(B7=4,ROUNDUP(F7/2,0),"N/A"))))</f>
         <v>N/A</v>
       </c>
-      <c r="F7" s="93"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="88" t="str">
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="23" t="str">
         <f t="shared" ref="I7:I11" si="1">IF(B7="P-.5",
 ODD((G7-C7)/H7),
 IF(B7="P-1",
@@ -2239,80 +2356,80 @@
         <v>PEDIDO DESCONOCIDO</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
-      <c r="B8" s="90"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="86" t="str">
+    <row r="8" spans="1:10" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="22" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
-      <c r="F8" s="93"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="88" t="str">
+      <c r="F8" s="68"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="23" t="str">
         <f t="shared" si="1"/>
         <v>PEDIDO DESCONOCIDO</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="86" t="str">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="22" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
-      <c r="F9" s="93"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="88" t="str">
+      <c r="F9" s="68"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="23" t="str">
         <f t="shared" si="1"/>
         <v>PEDIDO DESCONOCIDO</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="94"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="86" t="str">
+    <row r="10" spans="1:10" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="22" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
-      <c r="F10" s="96"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="88" t="str">
+      <c r="F10" s="70"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="23" t="str">
         <f t="shared" si="1"/>
         <v>PEDIDO DESCONOCIDO</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="97"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="86" t="str">
+    <row r="11" spans="1:10" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="22" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="88" t="str">
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="23" t="str">
         <f t="shared" si="1"/>
         <v>PEDIDO DESCONOCIDO</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B1:F2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:I3"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2425,7 +2542,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="17"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
@@ -2439,7 +2556,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="17"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
@@ -2453,7 +2570,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
@@ -2481,61 +2598,61 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>